<commit_message>
chg: version, dependency fixes
Mostly just tidying up after spending a while resolving problems whose
underlying cause was found in another library.
</commit_message>
<xml_diff>
--- a/tests/gui/empty_question_label_patch.xlsx
+++ b/tests/gui/empty_question_label_patch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="16380" windowHeight="7245" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="16380" windowHeight="7245" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>type</t>
   </si>
@@ -29,9 +29,6 @@
     <t>end group</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -53,16 +50,37 @@
     <t>a</t>
   </si>
   <si>
-    <t>My image label</t>
+    <t>text</t>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>item2</t>
+  </si>
+  <si>
+    <t>My image label 2</t>
+  </si>
+  <si>
+    <t>My image label 1</t>
+  </si>
+  <si>
+    <t>my_image2.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -115,8 +133,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -127,20 +145,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -266,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="survey" displayName="survey" ref="A1:D4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="survey" displayName="survey" ref="A1:D5" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D5"/>
   <tableColumns count="4">
     <tableColumn id="1" name="type" dataDxfId="3" dataCellStyle="Normal 2"/>
     <tableColumn id="2" name="name" dataDxfId="2" dataCellStyle="Normal 2"/>
@@ -650,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -673,49 +691,59 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
@@ -744,6 +772,10 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -760,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -771,18 +803,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>9</v>
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>